<commit_message>
tailings: add route A and B
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-sulfidic-tailings.xlsx
+++ b/premise/data/additional_inventories/lci-sulfidic-tailings.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahnme_a\PycharmProjects\premise\premise\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E0DCF4-11B3-4447-9654-FB9A809D969F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E931F9-9F22-4736-93B0-4F612B2476F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backfilling" sheetId="1" r:id="rId1"/>
+    <sheet name="flocculation-flotation" sheetId="2" r:id="rId2"/>
+    <sheet name="mwroasting_leaching" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="111">
   <si>
     <t>Database</t>
   </si>
@@ -212,14 +214,173 @@
     <t>US</t>
   </si>
   <si>
-    <t>ecoinvent_3.8</t>
+    <t>route_A</t>
+  </si>
+  <si>
+    <t>treatment of sulfidic tailings, flocculation-flotation process</t>
+  </si>
+  <si>
+    <t>Original inventory from Adrianto, L. R., &amp; Pfister, S. (2022). Prospective environmental assessment of reprocessing and valorization alternatives for sulfidic copper tailings. Resources, Conservation and Recycling, 186, 106567. https://doi.org/10.1016/j.resconrec.2022.106567</t>
+  </si>
+  <si>
+    <t>Adrianto, L. R., &amp; Pfister, S. (2022). Prospective environmental assessment of reprocessing and valorization alternatives for sulfidic copper tailings. Resources, Conservation and Recycling, 186, 106567. https://doi.org/10.1016/j.resconrec.2022.106567</t>
+  </si>
+  <si>
+    <t>The original dataset treats 1000kg of tailings, producing: 413kg aluminosilicate fraction (Si-Al) and 287kg of pyrite rich fraction. These can be use to produce CSA cement, ceramic tiles, or Portland cement. Hence, it is a multifunctional process (treatment of tailings + 2 products). Here, we do not model the use of the products downstream. Hence, following the cut-off approach, we attribute all environmental burderns to the treatment activity.
+Original inventory from Adrianto, L. R., &amp; Pfister, S. (2022). Prospective environmental assessment of reprocessing and valorization alternatives for sulfidic copper tailings. Resources, Conservation and Recycling, 186, 106567. https://doi.org/10.1016/j.resconrec.2022.106567</t>
+  </si>
+  <si>
+    <t>market for polyacrylamide</t>
+  </si>
+  <si>
+    <t>ecoinvent_3.8_cutoff</t>
+  </si>
+  <si>
+    <t>polyacrylamide</t>
+  </si>
+  <si>
+    <t>xanthate production</t>
+  </si>
+  <si>
+    <t>xanthate</t>
+  </si>
+  <si>
+    <t>treatment of wastewater, average, capacity 1E9l/year</t>
+  </si>
+  <si>
+    <t>wastewater, average</t>
+  </si>
+  <si>
+    <t>Original inventory treats 1 tonne of tailings</t>
+  </si>
+  <si>
+    <t>Original inventory produces 1 tonne of xanthate</t>
+  </si>
+  <si>
+    <t>carbon disulfide production</t>
+  </si>
+  <si>
+    <t>market for tap water</t>
+  </si>
+  <si>
+    <t>tap water</t>
+  </si>
+  <si>
+    <t>market for sodium hydroxide, without water, in 50% solution state</t>
+  </si>
+  <si>
+    <t>sodium hydroxide, without water, in 50% solution state</t>
+  </si>
+  <si>
+    <t>market for ethanol, without water, in 99.7% solution state, from ethylene</t>
+  </si>
+  <si>
+    <t>ethanol, without water, in 99.7% solution state, from ethylene</t>
+  </si>
+  <si>
+    <t>market for nitrogen, liquid</t>
+  </si>
+  <si>
+    <t>nitrogen, liquid</t>
+  </si>
+  <si>
+    <t>carbon disulfide</t>
+  </si>
+  <si>
+    <t>Original inventory based on Kunene et al. (2014).
+Inventory obtained from from Adrianto, L. R., &amp; Pfister, S. (2022). Prospective environmental assessment of reprocessing and valorization alternatives for sulfidic copper tailings. Resources, Conservation and Recycling, 186, 106567. https://doi.org/10.1016/j.resconrec.2022.106567</t>
+  </si>
+  <si>
+    <t>Original inventory produces 1 tonne of CS2</t>
+  </si>
+  <si>
+    <t>market group for heat, district or industrial, natural gas</t>
+  </si>
+  <si>
+    <t>megajoule</t>
+  </si>
+  <si>
+    <t>heat, district or industrial, natural gas</t>
+  </si>
+  <si>
+    <t>market for heat, from steam, in chemical industry</t>
+  </si>
+  <si>
+    <t>heat, from steam, in chemical industry</t>
+  </si>
+  <si>
+    <t>market group for tap water</t>
+  </si>
+  <si>
+    <t>natural gas production, low pressure, vehicle grade</t>
+  </si>
+  <si>
+    <t>RoW</t>
+  </si>
+  <si>
+    <t>natural gas, low pressure, vehicle grade</t>
+  </si>
+  <si>
+    <t>sulfur production, petroleum refinery operation</t>
+  </si>
+  <si>
+    <t>sulfur</t>
+  </si>
+  <si>
+    <t>market group for municipal solid waste</t>
+  </si>
+  <si>
+    <t>municipal solid waste</t>
+  </si>
+  <si>
+    <t>treatment of refinery sludge, hazardous waste incineration</t>
+  </si>
+  <si>
+    <t>refinery sludge</t>
+  </si>
+  <si>
+    <t>Sulfur dioxide</t>
+  </si>
+  <si>
+    <t>route_B</t>
+  </si>
+  <si>
+    <t>treatment of sulfidic tailings, roasting and leaching</t>
+  </si>
+  <si>
+    <t>The original dataset treats 1000kg of tailings, producing: 344.86 kg aluminosilicate fraction (Si-Al);  239.65 of PLS fraction; 68.97 of SO2; 4.05 kg of SO3; and surplus heat. These can be use to produce: ceramic tiles, or Portland cement (Al-Si fraction); and, metals or sulfuric acid. Hence, it is a multifunctional process (treatment of tailings + different products). Here, we do not model the use of the products downstream. Hence, following the cut-off approach, we attribute all environmental burderns to the treatment activity.
+Original inventory from Adrianto, L. R., &amp; Pfister, S. (2022). Prospective environmental assessment of reprocessing and valorization alternatives for sulfidic copper tailings. Resources, Conservation and Recycling, 186, 106567. https://doi.org/10.1016/j.resconrec.2022.106567</t>
+  </si>
+  <si>
+    <t>market for ammonia, anhydrous, liquid</t>
+  </si>
+  <si>
+    <t>ammonia, anhydrous, liquid</t>
+  </si>
+  <si>
+    <t>market for ammonium carbonate</t>
+  </si>
+  <si>
+    <t>ammonium carbonate</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Ammonium carbonate</t>
+  </si>
+  <si>
+    <t>tailings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +409,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,10 +438,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -832,7 +1003,7 @@
         <v>7.6E-3</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -855,7 +1026,7 @@
         <v>2.92E-2</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>57</v>
@@ -878,7 +1049,7 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -901,7 +1072,7 @@
         <v>6.2000000000000003E-5</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -924,7 +1095,7 @@
         <v>2.2000000000000001E-7</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
         <v>38</v>
@@ -947,7 +1118,7 @@
         <v>6.3399999999999999E-7</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
         <v>41</v>
@@ -970,7 +1141,7 @@
         <v>7.6000000000000003E-7</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
@@ -993,7 +1164,7 @@
         <v>1.08E-4</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
         <v>41</v>
@@ -1016,7 +1187,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
         <v>31</v>
@@ -1035,4 +1206,1224 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21FD9E9-61B0-485D-A6F2-E966007F3E24}">
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>B1</f>
+        <v>treatment of sulfidic tailings, flocculation-flotation process</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="str">
+        <f>B5</f>
+        <v>sulfidic tailings, generic</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <f>0.03/1000</f>
+        <v>2.9999999999999997E-5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <f>25.63/1000</f>
+        <v>2.563E-2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12">
+        <f>0.1/1000</f>
+        <v>1E-4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13">
+        <f>-0.3/1000</f>
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>B16</f>
+        <v>xanthate production</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" t="str">
+        <f>B20</f>
+        <v>xanthate</v>
+      </c>
+      <c r="I24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25">
+        <f>530/1000</f>
+        <v>0.53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <f>163.9/1000</f>
+        <v>0.16390000000000002</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27">
+        <f>1580/1000</f>
+        <v>1.58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28">
+        <f>280/1000</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29">
+        <f>320/1000</f>
+        <v>0.32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30">
+        <f>27.52/1000</f>
+        <v>2.7519999999999999E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>B33</f>
+        <v>carbon disulfide production</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" t="str">
+        <f>B37</f>
+        <v>carbon disulfide</v>
+      </c>
+      <c r="I41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <f>225/1000</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43">
+        <f>7510/1000</f>
+        <v>7.51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44">
+        <f>6540/1000</f>
+        <v>6.54</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45">
+        <f>1380/1000</f>
+        <v>1.38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46">
+        <f>224.02/1000</f>
+        <v>0.22402</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47">
+        <f>881.78/1000</f>
+        <v>0.88178000000000001</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48">
+        <f>-0.56/1000</f>
+        <v>-5.6000000000000006E-4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49">
+        <f>-1.86/1000</f>
+        <v>-1.8600000000000001E-3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50">
+        <f>-2.4/1000</f>
+        <v>-2.3999999999999998E-3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51">
+        <f>16.33/1000</f>
+        <v>1.6329999999999997E-2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52">
+        <f>40.5/1000</f>
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <f>362.36/1000</f>
+        <v>0.36236000000000002</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B10FDCC-BAED-4267-9C6F-A755C1FBA74B}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>B1</f>
+        <v>treatment of sulfidic tailings, roasting and leaching</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="str">
+        <f>B5</f>
+        <v>sulfidic tailings, generic</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <f>28.54/1000</f>
+        <v>2.8539999999999999E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11">
+        <f>228.79/1000</f>
+        <v>0.22878999999999999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12">
+        <f>1.99/1000</f>
+        <v>1.99E-3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13">
+        <f>5.61/1000</f>
+        <v>5.6100000000000004E-3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14">
+        <f>7.51/1000</f>
+        <v>7.5100000000000002E-3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15">
+        <f>584.5/1000</f>
+        <v>0.58450000000000002</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16">
+        <f>0.3/1000</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17">
+        <f>0.004/1000</f>
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18">
+        <f>0.0112/1000</f>
+        <v>1.1199999999999999E-5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>